<commit_message>
fix: stupid mistake in the 20th task
</commit_message>
<xml_diff>
--- a/Bariants/statgrad-ov-04-29/task_20.xlsx
+++ b/Bariants/statgrad-ov-04-29/task_20.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/htmlprogrammist/Python/ege/EGE/online-olimpiada-ov-04-29/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/htmlprogrammist/Python/ege/Bariants/statgrad-ov-04-29/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F473897B-091C-154E-A196-A404012BDAEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77A4EAA-F169-B240-B814-8C2D6A732A00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{4F857766-4BAF-2F4F-B65E-1E379EEE12EE}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140" xr2:uid="{4F857766-4BAF-2F4F-B65E-1E379EEE12EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -507,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DAB2A38-78F4-4240-84A1-49E29BF9868A}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -547,7 +547,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C4" s="2">
         <f>A4+1</f>
@@ -555,7 +555,7 @@
       </c>
       <c r="D4" s="2">
         <f>B4</f>
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E4" s="2">
         <f>C4+1</f>
@@ -563,15 +563,15 @@
       </c>
       <c r="F4" s="2">
         <f>D4</f>
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="G4" s="2">
-        <f>MAX(E4:F4)*2+MIN(E4:F4)</f>
-        <v>26</v>
+        <f>MAX(E4:F4)*3+MIN(E4:F4)</f>
+        <v>77</v>
       </c>
       <c r="H4">
         <f>SUM(E4:F4)</f>
-        <v>17</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -585,15 +585,15 @@
       </c>
       <c r="F5" s="2">
         <f>D4+1</f>
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="G5" s="2">
-        <f t="shared" ref="G5:G19" si="0">MAX(E5:F5)*2+MIN(E5:F5)</f>
-        <v>27</v>
+        <f t="shared" ref="G5:G19" si="0">MAX(E5:F5)*3+MIN(E5:F5)</f>
+        <v>79</v>
       </c>
       <c r="H5">
         <f t="shared" ref="H5:H19" si="1">SUM(E5:F5)</f>
-        <v>17</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -607,15 +607,15 @@
       </c>
       <c r="F6" s="2">
         <f>D4</f>
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="8" customFormat="1" ht="19" thickBot="1">
@@ -629,15 +629,15 @@
       </c>
       <c r="F7" s="6">
         <f>D4*3</f>
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
-        <v>61</v>
+        <v>214</v>
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -647,7 +647,7 @@
       </c>
       <c r="D8" s="5">
         <f>B4+1</f>
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="E8" s="5">
         <f>C8+1</f>
@@ -655,15 +655,15 @@
       </c>
       <c r="F8" s="5">
         <f>D8</f>
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -675,15 +675,15 @@
       </c>
       <c r="F9" s="2">
         <f>D8+1</f>
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="H9">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -695,15 +695,15 @@
       </c>
       <c r="F10" s="2">
         <f>D8</f>
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="H10">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="8" customFormat="1" ht="19" thickBot="1">
@@ -715,15 +715,15 @@
       </c>
       <c r="F11" s="6">
         <f>D8*3</f>
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="G11" s="2">
         <f t="shared" si="0"/>
-        <v>66</v>
+        <v>222</v>
       </c>
       <c r="H11">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -733,7 +733,7 @@
       </c>
       <c r="D12" s="5">
         <f>B4</f>
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E12" s="5">
         <f>C12+1</f>
@@ -741,15 +741,15 @@
       </c>
       <c r="F12" s="5">
         <f>D12</f>
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="G12" s="2">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="H12">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -761,15 +761,15 @@
       </c>
       <c r="F13" s="2">
         <f>D12+1</f>
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="G13" s="2">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="H13">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -781,15 +781,15 @@
       </c>
       <c r="F14" s="2">
         <f>D12</f>
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" si="0"/>
-        <v>117</v>
+        <v>185</v>
       </c>
       <c r="H14">
         <f t="shared" si="1"/>
-        <v>63</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="8" customFormat="1" ht="19" thickBot="1">
@@ -801,15 +801,15 @@
       </c>
       <c r="F15" s="6">
         <f>D12*3</f>
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" si="0"/>
-        <v>72</v>
+        <v>225</v>
       </c>
       <c r="H15">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -819,7 +819,7 @@
       </c>
       <c r="D16" s="5">
         <f>B4*3</f>
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="E16" s="5">
         <f>C16+1</f>
@@ -827,18 +827,18 @@
       </c>
       <c r="F16" s="5">
         <f>D16</f>
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="G16" s="2">
         <f t="shared" si="0"/>
-        <v>61</v>
+        <v>214</v>
       </c>
       <c r="H16">
         <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="3:8">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8">
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2">
@@ -847,18 +847,18 @@
       </c>
       <c r="F17" s="2">
         <f>D16+1</f>
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="G17" s="2">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>216</v>
       </c>
       <c r="H17">
         <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="3:8">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8">
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2">
@@ -867,18 +867,18 @@
       </c>
       <c r="F18" s="2">
         <f>D16</f>
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="G18" s="2">
         <f t="shared" si="0"/>
-        <v>72</v>
+        <v>225</v>
       </c>
       <c r="H18">
         <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="3:8" s="8" customFormat="1" ht="19" thickBot="1">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" s="8" customFormat="1" ht="19" thickBot="1">
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6">
@@ -887,15 +887,26 @@
       </c>
       <c r="F19" s="6">
         <f>D16*3</f>
-        <v>81</v>
+        <v>207</v>
       </c>
       <c r="G19" s="2">
         <f t="shared" si="0"/>
-        <v>168</v>
+        <v>627</v>
       </c>
       <c r="H19">
         <f t="shared" si="1"/>
-        <v>87</v>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>